<commit_message>
New Examples, little fix
</commit_message>
<xml_diff>
--- a/res_time.xlsx
+++ b/res_time.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\git\LogModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{54C05987-007D-4A85-9C2F-DB991A8AC95A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41420163-EACA-4620-8733-0FF00D45E764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="res_time" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1085,7 +1081,924 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>res_time!$C$19:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res_time!$A$19:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.61799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71870000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3495999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4623999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9123999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.521000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.0697999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.3428000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.428599999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.5855</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.946300000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.468500000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.772200000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.396699999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.4392</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-376D-4442-AF18-90D24D816EDD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>res_time!$C$19:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>res_time!$B$19:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.75280000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7970999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0783</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.076599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>308.36700000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-376D-4442-AF18-90D24D816EDD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="474271688"/>
+        <c:axId val="474273328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="474271688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474273328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="474273328"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474271688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Trv</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ"/>
+              <a:t>ání</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="cs-CZ" baseline="0"/>
+              <a:t> hledání (ms) v závislosti na počtu míst</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>res_time!$A$36:$A$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>0.79879999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8831</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9222999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.7835000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7321999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.363099999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.927600000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4093.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58.341299999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.014800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.0992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.0303</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>181.16800000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60.888800000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>42.659199999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>613.24800000000005</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>124.31399999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73.752700000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>134.41</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>280.86900000000003</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>98.116699999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D19-4B6B-9BA6-613BB7939241}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="374326888"/>
+        <c:axId val="374327872"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="374326888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374327872"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="374327872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374326888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1641,6 +2554,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1676,6 +3621,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90A5C87C-08EE-4E46-AB7D-AA50D1BC170E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>335280</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17F11306-DFAA-4D6E-A874-B5C7940E377F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1980,11 +3997,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2124,6 +4141,325 @@
         <v>16</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="B19">
+        <v>0.75280000000000002</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0.71870000000000001</v>
+      </c>
+      <c r="B20">
+        <v>1.7970999999999999</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1.3495999999999999</v>
+      </c>
+      <c r="B21">
+        <v>2.0783</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1.4623999999999999</v>
+      </c>
+      <c r="B22">
+        <v>32.076599999999999</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2.9123999999999999</v>
+      </c>
+      <c r="B23">
+        <v>308.36700000000002</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>12.521000000000001</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>5.0697999999999999</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>9.3428000000000004</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>15.428599999999999</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>14.5855</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>22.946300000000001</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>12.468500000000001</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>16.772200000000002</v>
+      </c>
+      <c r="C31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>24.396699999999999</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>37.4392</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0.79879999999999995</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0.9768</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0.8831</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>1.4398</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2.9222999999999999</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7.7835000000000001</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>5.7321999999999997</v>
+      </c>
+      <c r="C42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>12.363099999999999</v>
+      </c>
+      <c r="C43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>18.927600000000002</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4093.99</v>
+      </c>
+      <c r="C45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>58.341299999999997</v>
+      </c>
+      <c r="C46">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>17.014800000000001</v>
+      </c>
+      <c r="C47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>20.0992</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>18.0303</v>
+      </c>
+      <c r="C49">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>181.16800000000001</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>60.888800000000003</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>42.659199999999998</v>
+      </c>
+      <c r="C52">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>613.24800000000005</v>
+      </c>
+      <c r="C53">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>124.31399999999999</v>
+      </c>
+      <c r="C54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>73.752700000000004</v>
+      </c>
+      <c r="C55">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>134.41</v>
+      </c>
+      <c r="C56">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>280.86900000000003</v>
+      </c>
+      <c r="C57">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>98.116699999999994</v>
+      </c>
+      <c r="C58">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>